<commit_message>
Refs #8333 updated test data
</commit_message>
<xml_diff>
--- a/spec/test_data/census_employee_import/DCHL Employee Census 2.xlsx
+++ b/spec/test_data/census_employee_import/DCHL Employee Census 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nisanthyaganti/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nisanthyaganti/Documents/enroll/spec/test_data/census_employee_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Last Name</t>
   </si>
@@ -227,25 +227,7 @@
     <t>Zip(Optional)</t>
   </si>
   <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
     <t>DC Health Link  Employee Census Template</t>
-  </si>
-  <si>
-    <t>home</t>
   </si>
   <si>
     <r>
@@ -267,9 +249,6 @@
   </si>
   <si>
     <t>1.1</t>
-  </si>
-  <si>
-    <t>Date of Birth (DD/MM/YYYY)</t>
   </si>
   <si>
     <r>
@@ -296,7 +275,10 @@
     <t>Address Line 2(Optional)</t>
   </si>
   <si>
-    <t>abc123</t>
+    <t>Date of Birth (MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>Employee</t>
   </si>
   <si>
     <t>panther1</t>
@@ -308,7 +290,7 @@
     <t>abc</t>
   </si>
   <si>
-    <t>sr</t>
+    <t>Sr.</t>
   </si>
   <si>
     <t>111@gmail.com</t>
@@ -317,13 +299,25 @@
     <t>111111110</t>
   </si>
   <si>
-    <t>bf1</t>
+    <t>male</t>
   </si>
   <si>
-    <t>100 NY Avenue</t>
+    <t>no</t>
   </si>
   <si>
-    <t xml:space="preserve">Washington </t>
+    <t>home</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>bf1</t>
   </si>
   <si>
     <t>runner1</t>
@@ -333,6 +327,12 @@
   </si>
   <si>
     <t>111-22-9990</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>yuteir7685</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1036,6 +1036,10 @@
     <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="79">
     <cellStyle name="20% - Accent1 2" xfId="4"/>
@@ -1118,27 +1122,7 @@
     <cellStyle name="Total 2" xfId="55"/>
     <cellStyle name="Warning Text 2" xfId="56"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1475,9 +1459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U410"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1505,7 +1489,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="20" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1522,7 +1506,7 @@
       <c r="L1" s="19"/>
       <c r="M1" s="23"/>
       <c r="N1" s="22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:21" customFormat="1" ht="31.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1578,7 +1562,7 @@
         <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
         <v>28</v>
@@ -1592,7 +1576,7 @@
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>5</v>
@@ -1613,10 +1597,10 @@
         <v>2</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>18</v>
@@ -1643,7 +1627,7 @@
         <v>33</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="S3" s="33" t="s">
         <v>34</v>
@@ -1657,41 +1641,41 @@
     </row>
     <row r="4" spans="1:21" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="I4" s="5">
         <v>14699</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="K4" s="6">
         <v>40695</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="N4" s="8" t="s">
         <v>57</v>
@@ -1700,16 +1684,19 @@
         <v>2016</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="U4" s="9">
         <v>20001</v>
@@ -1717,30 +1704,32 @@
     </row>
     <row r="5" spans="1:21" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="35"/>
       <c r="H5" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I5" s="5">
         <v>36249</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="M5" s="36"/>
+      <c r="M5" s="36" t="s">
+        <v>52</v>
+      </c>
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:21" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1749,14 +1738,14 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="35"/>
       <c r="H6" s="7"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="36"/>
+      <c r="J6" s="24"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="36"/>
+      <c r="M6" s="3"/>
       <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:21" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6809,39 +6798,35 @@
       <c r="N410" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H7:H14">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="H6:H14">
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
+  <conditionalFormatting sqref="H4">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H5">
+  <conditionalFormatting sqref="H5">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B1048576 B8 B10 B12 B14 B1:B4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B4 B6 B8 B10 B12 B14 B16:B1048576">
       <formula1>"Employee,Spouse,Domestic Partner,Child"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P7:P61 P4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P61">
       <formula1>"home,work"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B5:B7 B9 B11 B13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B7 B9 B11 B13">
       <formula1>"Employee,Spouse,Domestic Partner,Child,Disabled Child"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="ACH7:ACH302 AMD7:AMD302 AVZ7:AVZ302 BFV7:BFV302 BPR7:BPR302 BZN7:BZN302 CJJ7:CJJ302 CTF7:CTF302 DDB7:DDB302 DMX7:DMX302 DWT7:DWT302 EGP7:EGP302 EQL7:EQL302 FAH7:FAH302 FKD7:FKD302 FTZ7:FTZ302 GDV7:GDV302 GNR7:GNR302 GXN7:GXN302 HHJ7:HHJ302 HRF7:HRF302 IBB7:IBB302 IKX7:IKX302 IUT7:IUT302 JEP7:JEP302 JOL7:JOL302 JYH7:JYH302 KID7:KID302 KRZ7:KRZ302 LBV7:LBV302 LLR7:LLR302 LVN7:LVN302 MFJ7:MFJ302 MPF7:MPF302 MZB7:MZB302 NIX7:NIX302 NST7:NST302 OCP7:OCP302 OML7:OML302 OWH7:OWH302 PGD7:PGD302 PPZ7:PPZ302 PZV7:PZV302 QJR7:QJR302 QTN7:QTN302 RDJ7:RDJ302 RNF7:RNF302 RXB7:RXB302 SGX7:SGX302 SQT7:SQT302 TAP7:TAP302 TKL7:TKL302 TUH7:TUH302 UED7:UED302 UNZ7:UNZ302 UXV7:UXV302 VHR7:VHR302 VRN7:VRN302 WBJ7:WBJ302 WLF7:WLF302 WVB7:WVB302 IP7:IP302 SL7:SL302 IO4:IO6 SK4:SK6 ACG4:ACG6 AMC4:AMC6 AVY4:AVY6 BFU4:BFU6 BPQ4:BPQ6 BZM4:BZM6 CJI4:CJI6 CTE4:CTE6 DDA4:DDA6 DMW4:DMW6 DWS4:DWS6 EGO4:EGO6 EQK4:EQK6 FAG4:FAG6 FKC4:FKC6 FTY4:FTY6 GDU4:GDU6 GNQ4:GNQ6 GXM4:GXM6 HHI4:HHI6 HRE4:HRE6 IBA4:IBA6 IKW4:IKW6 IUS4:IUS6 JEO4:JEO6 JOK4:JOK6 JYG4:JYG6 KIC4:KIC6 KRY4:KRY6 LBU4:LBU6 LLQ4:LLQ6 LVM4:LVM6 MFI4:MFI6 MPE4:MPE6 MZA4:MZA6 NIW4:NIW6 NSS4:NSS6 OCO4:OCO6 OMK4:OMK6 OWG4:OWG6 PGC4:PGC6 PPY4:PPY6 PZU4:PZU6 QJQ4:QJQ6 QTM4:QTM6 RDI4:RDI6 RNE4:RNE6 RXA4:RXA6 SGW4:SGW6 SQS4:SQS6 TAO4:TAO6 TKK4:TKK6 TUG4:TUG6 UEC4:UEC6 UNY4:UNY6 UXU4:UXU6 VHQ4:VHQ6 VRM4:VRM6 WBI4:WBI6 WLE4:WLE6 WVA4:WVA6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="IP4:IP302 SL4:SL302 ACH4:ACH302 AMD4:AMD302 AVZ4:AVZ302 BFV4:BFV302 BPR4:BPR302 BZN4:BZN302 CJJ4:CJJ302 CTF4:CTF302 DDB4:DDB302 DMX4:DMX302 DWT4:DWT302 EGP4:EGP302 EQL4:EQL302 FAH4:FAH302 FKD4:FKD302 FTZ4:FTZ302 GDV4:GDV302 GNR4:GNR302 GXN4:GXN302 HHJ4:HHJ302 HRF4:HRF302 IBB4:IBB302 IKX4:IKX302 IUT4:IUT302 JEP4:JEP302 JOL4:JOL302 JYH4:JYH302 KID4:KID302 KRZ4:KRZ302 LBV4:LBV302 LLR4:LLR302 LVN4:LVN302 MFJ4:MFJ302 MPF4:MPF302 MZB4:MZB302 NIX4:NIX302 NST4:NST302 OCP4:OCP302 OML4:OML302 OWH4:OWH302 PGD4:PGD302 PPZ4:PPZ302 PZV4:PZV302 QJR4:QJR302 QTN4:QTN302 RDJ4:RDJ302 RNF4:RNF302 RXB4:RXB302 SGX4:SGX302 SQT4:SQT302 TAP4:TAP302 TKL4:TKL302 TUH4:TUH302 UED4:UED302 UNZ4:UNZ302 UXV4:UXV302 VHR4:VHR302 VRN4:VRN302 WBJ4:WBJ302 WLF4:WLF302 WVB4:WVB302">
       <formula1>EERelationships</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IT7:IT302 SP7:SP302 ACL7:ACL302 AMH7:AMH302 AWD7:AWD302 BFZ7:BFZ302 BPV7:BPV302 BZR7:BZR302 CJN7:CJN302 CTJ7:CTJ302 DDF7:DDF302 DNB7:DNB302 DWX7:DWX302 EGT7:EGT302 EQP7:EQP302 FAL7:FAL302 FKH7:FKH302 FUD7:FUD302 GDZ7:GDZ302 GNV7:GNV302 GXR7:GXR302 HHN7:HHN302 HRJ7:HRJ302 IBF7:IBF302 ILB7:ILB302 IUX7:IUX302 JET7:JET302 JOP7:JOP302 JYL7:JYL302 KIH7:KIH302 KSD7:KSD302 LBZ7:LBZ302 LLV7:LLV302 LVR7:LVR302 MFN7:MFN302 MPJ7:MPJ302 MZF7:MZF302 NJB7:NJB302 NSX7:NSX302 OCT7:OCT302 OMP7:OMP302 OWL7:OWL302 PGH7:PGH302 PQD7:PQD302 PZZ7:PZZ302 QJV7:QJV302 QTR7:QTR302 RDN7:RDN302 RNJ7:RNJ302 RXF7:RXF302 SHB7:SHB302 SQX7:SQX302 TAT7:TAT302 TKP7:TKP302 TUL7:TUL302 UEH7:UEH302 UOD7:UOD302 UXZ7:UXZ302 VHV7:VHV302 VRR7:VRR302 WBN7:WBN302 WLJ7:WLJ302 WVF7:WVF302 F4:F6 WVE4:WVE6 IS4:IS6 SO4:SO6 ACK4:ACK6 AMG4:AMG6 AWC4:AWC6 BFY4:BFY6 BPU4:BPU6 BZQ4:BZQ6 CJM4:CJM6 CTI4:CTI6 DDE4:DDE6 DNA4:DNA6 DWW4:DWW6 EGS4:EGS6 EQO4:EQO6 FAK4:FAK6 FKG4:FKG6 FUC4:FUC6 GDY4:GDY6 GNU4:GNU6 GXQ4:GXQ6 HHM4:HHM6 HRI4:HRI6 IBE4:IBE6 ILA4:ILA6 IUW4:IUW6 JES4:JES6 JOO4:JOO6 JYK4:JYK6 KIG4:KIG6 KSC4:KSC6 LBY4:LBY6 LLU4:LLU6 LVQ4:LVQ6 MFM4:MFM6 MPI4:MPI6 MZE4:MZE6 NJA4:NJA6 NSW4:NSW6 OCS4:OCS6 OMO4:OMO6 OWK4:OWK6 PGG4:PGG6 PQC4:PQC6 PZY4:PZY6 QJU4:QJU6 QTQ4:QTQ6 RDM4:RDM6 RNI4:RNI6 RXE4:RXE6 SHA4:SHA6 SQW4:SQW6 TAS4:TAS6 TKO4:TKO6 TUK4:TUK6 UEG4:UEG6 UOC4:UOC6 UXY4:UXY6 VHU4:VHU6 VRQ4:VRQ6 WBM4:WBM6 WLI4:WLI6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WLJ4:WLJ302 WVF4:WVF302 IT4:IT302 SP4:SP302 ACL4:ACL302 AMH4:AMH302 AWD4:AWD302 BFZ4:BFZ302 BPV4:BPV302 BZR4:BZR302 CJN4:CJN302 CTJ4:CTJ302 DDF4:DDF302 DNB4:DNB302 DWX4:DWX302 EGT4:EGT302 EQP4:EQP302 FAL4:FAL302 FKH4:FKH302 FUD4:FUD302 GDZ4:GDZ302 GNV4:GNV302 GXR4:GXR302 HHN4:HHN302 HRJ4:HRJ302 IBF4:IBF302 ILB4:ILB302 IUX4:IUX302 JET4:JET302 JOP4:JOP302 JYL4:JYL302 KIH4:KIH302 KSD4:KSD302 LBZ4:LBZ302 LLV4:LLV302 LVR4:LVR302 MFN4:MFN302 MPJ4:MPJ302 MZF4:MZF302 NJB4:NJB302 NSX4:NSX302 OCT4:OCT302 OMP4:OMP302 OWL4:OWL302 PGH4:PGH302 PQD4:PQD302 PZZ4:PZZ302 QJV4:QJV302 QTR4:QTR302 RDN4:RDN302 RNJ4:RNJ302 RXF4:RXF302 SHB4:SHB302 SQX4:SQX302 TAT4:TAT302 TKP4:TKP302 TUL4:TUL302 UEH4:UEH302 UOD4:UOD302 UXZ4:UXZ302 VHV4:VHV302 VRR4:VRR302 WBN4:WBN302">
       <formula1>Suffix</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="ACQ7:ACR302 AMM7:AMN302 AWI7:AWJ302 BGE7:BGF302 BQA7:BQB302 BZW7:BZX302 CJS7:CJT302 CTO7:CTP302 DDK7:DDL302 DNG7:DNH302 DXC7:DXD302 EGY7:EGZ302 EQU7:EQV302 FAQ7:FAR302 FKM7:FKN302 FUI7:FUJ302 GEE7:GEF302 GOA7:GOB302 GXW7:GXX302 HHS7:HHT302 HRO7:HRP302 IBK7:IBL302 ILG7:ILH302 IVC7:IVD302 JEY7:JEZ302 JOU7:JOV302 JYQ7:JYR302 KIM7:KIN302 KSI7:KSJ302 LCE7:LCF302 LMA7:LMB302 LVW7:LVX302 MFS7:MFT302 MPO7:MPP302 MZK7:MZL302 NJG7:NJH302 NTC7:NTD302 OCY7:OCZ302 OMU7:OMV302 OWQ7:OWR302 PGM7:PGN302 PQI7:PQJ302 QAE7:QAF302 QKA7:QKB302 QTW7:QTX302 RDS7:RDT302 RNO7:RNP302 RXK7:RXL302 SHG7:SHH302 SRC7:SRD302 TAY7:TAZ302 TKU7:TKV302 TUQ7:TUR302 UEM7:UEN302 UOI7:UOJ302 UYE7:UYF302 VIA7:VIB302 VRW7:VRX302 WBS7:WBT302 WLO7:WLP302 WVK7:WVL302 IY7:IZ302 SU7:SV302 IX4:IY6 ST4:SU6 ACP4:ACQ6 AML4:AMM6 AWH4:AWI6 BGD4:BGE6 BPZ4:BQA6 BZV4:BZW6 CJR4:CJS6 CTN4:CTO6 DDJ4:DDK6 DNF4:DNG6 DXB4:DXC6 EGX4:EGY6 EQT4:EQU6 FAP4:FAQ6 FKL4:FKM6 FUH4:FUI6 GED4:GEE6 GNZ4:GOA6 GXV4:GXW6 HHR4:HHS6 HRN4:HRO6 IBJ4:IBK6 ILF4:ILG6 IVB4:IVC6 JEX4:JEY6 JOT4:JOU6 JYP4:JYQ6 KIL4:KIM6 KSH4:KSI6 LCD4:LCE6 LLZ4:LMA6 LVV4:LVW6 MFR4:MFS6 MPN4:MPO6 MZJ4:MZK6 NJF4:NJG6 NTB4:NTC6 OCX4:OCY6 OMT4:OMU6 OWP4:OWQ6 PGL4:PGM6 PQH4:PQI6 QAD4:QAE6 QJZ4:QKA6 QTV4:QTW6 RDR4:RDS6 RNN4:RNO6 RXJ4:RXK6 SHF4:SHG6 SRB4:SRC6 TAX4:TAY6 TKT4:TKU6 TUP4:TUQ6 UEL4:UEM6 UOH4:UOI6 UYD4:UYE6 VHZ4:VIA6 VRV4:VRW6 WBR4:WBS6 WLN4:WLO6 WVJ4:WVK6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="IY4:IZ302 SU4:SV302 ACQ4:ACR302 AMM4:AMN302 AWI4:AWJ302 BGE4:BGF302 BQA4:BQB302 BZW4:BZX302 CJS4:CJT302 CTO4:CTP302 DDK4:DDL302 DNG4:DNH302 DXC4:DXD302 EGY4:EGZ302 EQU4:EQV302 FAQ4:FAR302 FKM4:FKN302 FUI4:FUJ302 GEE4:GEF302 GOA4:GOB302 GXW4:GXX302 HHS4:HHT302 HRO4:HRP302 IBK4:IBL302 ILG4:ILH302 IVC4:IVD302 JEY4:JEZ302 JOU4:JOV302 JYQ4:JYR302 KIM4:KIN302 KSI4:KSJ302 LCE4:LCF302 LMA4:LMB302 LVW4:LVX302 MFS4:MFT302 MPO4:MPP302 MZK4:MZL302 NJG4:NJH302 NTC4:NTD302 OCY4:OCZ302 OMU4:OMV302 OWQ4:OWR302 PGM4:PGN302 PQI4:PQJ302 QAE4:QAF302 QKA4:QKB302 QTW4:QTX302 RDS4:RDT302 RNO4:RNP302 RXK4:RXL302 SHG4:SHH302 SRC4:SRD302 TAY4:TAZ302 TKU4:TKV302 TUQ4:TUR302 UEM4:UEN302 UOI4:UOJ302 UYE4:UYF302 VIA4:VIB302 VRW4:VRX302 WBS4:WBT302 WLO4:WLP302 WVK4:WVL302">
       <formula1>Status</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="date" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter date of birth between 1/1/1920 and today" sqref="I1:I2 I7:I1048576">
-      <formula1>7306</formula1>
-      <formula2>TODAY()</formula2>
     </dataValidation>
     <dataValidation operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:L1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
@@ -6850,12 +6835,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
       <formula1>"male,female"</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter date of birth between 1/1/1920 and today" sqref="I3:I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>"Jr., Sr., II, III, IV, V"</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I3 I6:I1048576">
       <formula1>7306</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F3 F7:F1048576">
-      <formula1>"Jr., Sr., II, III, IV, V"</formula1>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter date of birth between 1/1/1920 and today" sqref="I4:I5">
+      <formula1>7306</formula1>
+      <formula2>TODAY()</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>